<commit_message>
evaluation task, trial generation for it, changes to surveillance task size
</commit_message>
<xml_diff>
--- a/measures/instructions.xlsx
+++ b/measures/instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/unconscious-ec-RRR/measures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DA1D12F-9929-EF4E-9434-831531B7467A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257A761F-E0C6-9B4C-9A4C-449AC89D9B74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7220" yWindow="460" windowWidth="26820" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5180" yWindow="460" windowWidth="26820" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Imagine that you are a security guard watching for deviant activity at a business. Your job requires that you pay attention at all times, and respond quickly when something suspicious happens.  
 In our lab we study attention and rapid responding, and in this experiment you'll be asked to play the role of the security guard. 
@@ -54,6 +54,23 @@
   <si>
     <t>For each of the following statements please indicate to what extent they are characteristic of you.
 Please note that there are no right or wrong answers.</t>
+  </si>
+  <si>
+    <t>Next, you'll be presented with 30 pairs of target and filler creatures from the surveillance tasks, and we'd like you to indicate which one you like better. 
+You don't need a reason for liking one rather than the other, just give us your gut feelings.
+We are interested in knowing if the pleasantness or unpleasantness of these stimuli affects the ability to attend and rapidly respond to them, so we need you to indicate which you prefer.  
+Remember, you don't need a reason for liking one rather than the other, so just go with your gut. Please respond quickly.
+Press the spacebar to continue.</t>
+  </si>
+  <si>
+    <t>Put a left finger on the E key and a right finger in the I key.
+If you prefer the creature on the left, press E.
+If you prefer the creature on the right, press I.
+Press the spacebar to continue.</t>
+  </si>
+  <si>
+    <t>The experiment is now complete.
+Press the spacebar to finish.</t>
   </si>
 </sst>
 </file>
@@ -549,9 +566,8 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -921,8 +937,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,48 +947,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="220" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="297" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
+      <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="230" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A6" s="5" t="s">
+      <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A7" s="5" t="s">
+      <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
+    <row r="8" spans="1:1" ht="221" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
+    <row r="9" spans="1:1" ht="136" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>8</v>
+      </c>
     </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="1"/>
+    <row r="10" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>9</v>
+      </c>
     </row>
   </sheetData>
   <sheetProtection sheet="1" objects="1" scenarios="1"/>

</xml_diff>

<commit_message>
added awareness quesitons, corrected surveillance instructions,
</commit_message>
<xml_diff>
--- a/measures/instructions.xlsx
+++ b/measures/instructions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Ian/git/unconscious-ec-RRR/measures/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257A761F-E0C6-9B4C-9A4C-449AC89D9B74}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BDA9CF-19A5-234F-95AD-F5B137D609C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="460" windowWidth="26820" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1980" yWindow="460" windowWidth="26820" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="instructions" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Imagine that you are a security guard watching for deviant activity at a business. Your job requires that you pay attention at all times, and respond quickly when something suspicious happens.  
 In our lab we study attention and rapid responding, and in this experiment you'll be asked to play the role of the security guard. 
@@ -71,6 +71,10 @@
   <si>
     <t>The experiment is now complete.
 Press the spacebar to finish.</t>
+  </si>
+  <si>
+    <t>Lastly, we'll ask you a small number of questions, and then the study will end.
+Press the spacebar to continue.</t>
   </si>
 </sst>
 </file>
@@ -566,7 +570,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="34" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
@@ -578,6 +582,14 @@
     </xf>
     <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -935,10 +947,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:A10"/>
+  <dimension ref="A1:A11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -991,8 +1003,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:1" ht="51" x14ac:dyDescent="0.2">
-      <c r="A10" s="4" t="s">
+    <row r="10" spans="1:1" ht="75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A10" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" ht="51" x14ac:dyDescent="0.2">
+      <c r="A11" s="5" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>